<commit_message>
chore: generate Jekyll collections from Google Sheet
</commit_message>
<xml_diff>
--- a/data/luismcsoul_content_updated.xlsx
+++ b/data/luismcsoul_content_updated.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M139"/>
+  <dimension ref="A1:N139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>citation</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>body_md</t>
         </is>
       </c>
@@ -529,7 +534,8 @@
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr">
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
         <is>
           <t>Revengeful trading,
  our lives.</t>
@@ -577,7 +583,8 @@
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr">
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
         <is>
           <t>Amazing
  always
@@ -627,7 +634,8 @@
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
         <is>
           <t>Deconspire
  yourself.</t>
@@ -671,7 +679,8 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
         <is>
           <t>Broken things
  bear my name.</t>
@@ -715,7 +724,8 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
         <is>
           <t>In the place 
  where he died,
@@ -768,7 +778,8 @@
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
         <is>
           <t>To paradise 
  we don't arrive, 
@@ -813,7 +824,8 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
         <is>
           <t>The flies 
  know 
@@ -859,7 +871,8 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr">
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
         <is>
           <t>Behind
  every evil woman,
@@ -905,7 +918,8 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
         <is>
           <t>They were
  four kings,
@@ -951,7 +965,8 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr">
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
         <is>
           <t>Dan Overcash
  is always broke.</t>
@@ -995,7 +1010,8 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
         <is>
           <t>Let's play it 
  our way
@@ -1040,7 +1056,8 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
         <is>
           <t>A battery
  increases his size
@@ -1087,7 +1104,8 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
         <is>
           <t>In the living room
  I have now
@@ -1133,7 +1151,8 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
         <is>
           <t>Two seconds ago
  this river wasn't here.</t>
@@ -1177,7 +1196,8 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr">
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
         <is>
           <t>Mummies
  digitally
@@ -1222,7 +1242,8 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
         <is>
           <t>During starry nights, 
  remember always to spot
@@ -1267,7 +1288,8 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
         <is>
           <t>Attention is a currency,
  you always must 
@@ -1312,7 +1334,8 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
         <is>
           <t>For the photon,
  we are still photography.</t>
@@ -1356,7 +1379,8 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr">
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
         <is>
           <t>A house is not a home,
  if you are not welcome.</t>
@@ -1400,7 +1424,8 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr">
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
         <is>
           <t>Don't wait 
  "for the pain to make sense"</t>
@@ -1444,7 +1469,8 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr">
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
         <is>
           <t>A missing piece,
  makes obsolete
@@ -1491,6 +1517,13 @@
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
+          <t>Neil Peart, 
+Rush, 
+Supercoductor.</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
           <t>Reverse Engineer
  "the fantasies that you romance to"</t>
         </is>
@@ -1533,7 +1566,8 @@
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr">
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
         <is>
           <t>Messenger
  and Message
@@ -1578,7 +1612,8 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr">
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
         <is>
           <t>Opium wars
  backfire.</t>
@@ -1622,7 +1657,8 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr">
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
         <is>
           <t>Deliver us
  from anything
@@ -1668,7 +1704,8 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr">
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
         <is>
           <t>A basketball's free throw
  never lies.</t>
@@ -1712,7 +1749,8 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr">
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
         <is>
           <t>A gun
  that retrogrades
@@ -1758,7 +1796,8 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr">
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
         <is>
           <t>Wish
  that the person 
@@ -1805,7 +1844,8 @@
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr">
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
         <is>
           <t>Symmetry
  is mirrored
@@ -1850,7 +1890,8 @@
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr">
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr">
         <is>
           <t>If the audience is too big,
  nothing important
@@ -1895,7 +1936,8 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr">
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
         <is>
           <t>Virus
  database
@@ -1941,7 +1983,8 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr">
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
         <is>
           <t>NEWBORN GAZE:
  The universe
@@ -1986,7 +2029,8 @@
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr">
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
         <is>
           <t>BUILDING:
  A cuboid mount
@@ -2035,7 +2079,8 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr">
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
         <is>
           <t>PENCIL:
  Ashes reincarnating
@@ -2081,7 +2126,8 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr">
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
         <is>
           <t>INNER EAR:
  A living fossil
@@ -2126,7 +2172,8 @@
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr">
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
         <is>
           <t>ANTICIPATION:
  One thousand
@@ -2173,7 +2220,8 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr">
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr">
         <is>
           <t>ASSESSMENT:
  The way dogs 
@@ -2219,7 +2267,8 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr">
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
         <is>
           <t>BODYBUILDER:
  She wears her skin.</t>
@@ -2263,7 +2312,8 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr">
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
         <is>
           <t>SOCIAL MEDIAS:
  Memories
@@ -2317,7 +2367,8 @@
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr">
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
         <is>
           <t>EINSTEIN
  (hindrance):
@@ -2362,7 +2413,8 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr">
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
         <is>
           <t>PLANTS:
  Under Earth as it is in Heaven,
@@ -2409,7 +2461,8 @@
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr">
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr">
         <is>
           <t>MUSE/MUSIC:
  Heartbeat
@@ -2458,6 +2511,11 @@
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
+          <t>Google Maps</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
           <t>GENTRIFICATION:
  "Customise your driving avatar"</t>
         </is>
@@ -2500,7 +2558,8 @@
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr">
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr">
         <is>
           <t>STATIC BICYCLE:
  A ride
@@ -2545,7 +2604,8 @@
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr">
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr">
         <is>
           <t>VERTEBRAE:
  Column,
@@ -2591,7 +2651,8 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr">
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr">
         <is>
           <t>INTELLIGENCE:
  Inversely proportionate
@@ -2637,7 +2698,8 @@
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr">
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr">
         <is>
           <t>CANIS MAJOR:
  Collective Unconsciousness,
@@ -2683,7 +2745,8 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr">
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr">
         <is>
           <t>SPIRIT:
  When the animal stops,
@@ -2728,7 +2791,8 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr">
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr">
         <is>
           <t>ID BADGE:
  The heaviest object
@@ -2773,7 +2837,8 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr">
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr">
         <is>
           <t>IN THE RIVER
  All stones are rounded by time.
@@ -2819,7 +2884,8 @@
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr">
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr">
         <is>
           <t>GRAVE MARKERS
  With only full names
@@ -2866,7 +2932,8 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr">
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
         <is>
           <t>CINDERELLA
  Goes to sleep
@@ -2914,7 +2981,8 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr">
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr">
         <is>
           <t>PROPORTIONAL
  Followers of shiny things
@@ -2960,7 +3028,8 @@
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr">
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
         <is>
           <t>WEIGHT
  After scanning the whole store 
@@ -3008,7 +3077,8 @@
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr">
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr">
         <is>
           <t>SLEEPING BAG
  This anaconda,
@@ -3054,7 +3124,8 @@
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr">
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr">
         <is>
           <t>THE SLAVES
  Were finally free
@@ -3101,7 +3172,8 @@
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr">
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr">
         <is>
           <t>INFINITY
  From this perspective
@@ -3147,7 +3219,8 @@
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr">
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr">
         <is>
           <t>EVERY NUMBER
  Every number is 
@@ -3194,7 +3267,8 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr">
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr">
         <is>
           <t>THE BACTERIA
  Inside our guts
@@ -3241,7 +3315,8 @@
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr">
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr">
         <is>
           <t>LOOK AROUND
  All metal, glass, plastic and concrete,
@@ -3291,7 +3366,8 @@
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr">
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr">
         <is>
           <t>ORCHESTRA
  Groups of women 
@@ -3340,7 +3416,8 @@
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
-      <c r="M63" t="inlineStr">
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr">
         <is>
           <t>A CHINESE EMPEROR
  died
@@ -3389,6 +3466,11 @@
       <c r="L64" t="inlineStr"/>
       <c r="M64" t="inlineStr">
         <is>
+          <t>Edgar Allan Poe</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
           <t>EVERYWHERE I LOOK
  "The Masque of the Red Death"</t>
         </is>
@@ -3431,7 +3513,8 @@
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr">
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr">
         <is>
           <t>A SMALL TIE
  Is a perfect coat
@@ -3476,7 +3559,8 @@
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr">
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr">
         <is>
           <t>SANS-SOUCI
  "Care-free"
@@ -3522,7 +3606,8 @@
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr"/>
-      <c r="M67" t="inlineStr">
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr">
         <is>
           <t>FROM RED TO GREEN
  There are 
@@ -3568,7 +3653,8 @@
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr">
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr">
         <is>
           <t>BITCOIN WAS THE TEST NET
  For a further 
@@ -3614,7 +3700,8 @@
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr"/>
-      <c r="M69" t="inlineStr">
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr">
         <is>
           <t>IN THE TEMPLE
  Days of endless mantras
@@ -3659,7 +3746,8 @@
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr">
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr">
         <is>
           <t>SISYPHUS SYZIGY
  Each one of us 
@@ -3708,7 +3796,8 @@
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
-      <c r="M71" t="inlineStr">
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr">
         <is>
           <t>I'M FULL OF SUPERSTITION
  as scientificaly backed
@@ -3753,7 +3842,8 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr">
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr">
         <is>
           <t>YOUR SALARY
  is still
@@ -3800,7 +3890,8 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr">
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr">
         <is>
           <t>SEAMLESSLY
  Wherever you see 
@@ -3847,7 +3938,8 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr">
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr">
         <is>
           <t>I KNOW ABOUT HAPPINESS
  Because 
@@ -3893,7 +3985,8 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr">
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr">
         <is>
           <t>COUNTERINTUITIVE
  Removing temptations
@@ -3938,7 +4031,8 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr">
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr">
         <is>
           <t>IN A CASINO
  I lost everything
@@ -3984,7 +4078,8 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr">
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr">
         <is>
           <t>ARTIFICIAL INTELLIGENCE
  Has revealed:
@@ -4030,7 +4125,8 @@
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr">
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr">
         <is>
           <t>MIND WHERE YOU ARE
  Convergent evolution
@@ -4075,7 +4171,8 @@
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr">
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr">
         <is>
           <t>IKARIA WARIOOTIA
  Inside of us all,
@@ -4123,7 +4220,8 @@
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr">
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr">
         <is>
           <t>DEEP SLEEP
  Requires
@@ -4169,7 +4267,8 @@
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr">
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr">
         <is>
           <t>BY THE CUT
  See you
@@ -4216,7 +4315,8 @@
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr">
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr">
         <is>
           <t>DOWN IN THE HORIZON
  Sirius blinks red, white and blue,
@@ -4262,7 +4362,8 @@
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
-      <c r="M83" t="inlineStr">
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr">
         <is>
           <t>SUCCESSOR
  Depends on
@@ -4308,7 +4409,8 @@
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr">
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr">
         <is>
           <t>THE CELLS
  That could understand
@@ -4356,7 +4458,8 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr">
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr">
         <is>
           <t>YOU CAN'T GO BACK IN TIME
  But you can move forward
@@ -4404,7 +4507,8 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
-      <c r="M86" t="inlineStr">
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr">
         <is>
           <t>ONCE I SAT DOWN
  In Zen Meditation.
@@ -4452,7 +4556,8 @@
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr">
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr">
         <is>
           <t>TAO
  Mistery and Mastery
@@ -4502,6 +4607,11 @@
       <c r="L88" t="inlineStr"/>
       <c r="M88" t="inlineStr">
         <is>
+          <t>Arthur C. Clarke</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
           <t>COMMIT
  Humans 'will not longer commute',
  neither 'they will communicate'
@@ -4550,7 +4660,8 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr">
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr">
         <is>
           <t>TRANSCENDENTAL
  Imaginary Time
@@ -4604,7 +4715,8 @@
       </c>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr">
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr">
         <is>
           <t>"I" BEARS THE SHADOW
  The sun dances
@@ -4658,7 +4770,8 @@
       </c>
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr">
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr">
         <is>
           <t>MOUNTAINS
  Are destroyed
@@ -4712,7 +4825,8 @@
       </c>
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr">
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr">
         <is>
           <t>SHARING THE SAME DNA
  We are all subjects to
@@ -4758,7 +4872,8 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr">
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr">
         <is>
           <t>TIME STAMPS
  Work in progress
@@ -4811,7 +4926,8 @@
       </c>
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr">
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr">
         <is>
           <t>OUR MEMORIES
  Are being overwritten
@@ -4856,7 +4972,8 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr">
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr">
         <is>
           <t>THE ANTS CAME
  and took away, 
@@ -4915,7 +5032,8 @@
         </is>
       </c>
       <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr">
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr">
         <is>
           <t>Scrolling
  down
@@ -4972,7 +5090,8 @@
         </is>
       </c>
       <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr">
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr">
         <is>
           <t>Wish to have no followers</t>
         </is>
@@ -5027,7 +5146,8 @@
         </is>
       </c>
       <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr">
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr">
         <is>
           <t>SOUND MINDED
  ✳</t>
@@ -5083,7 +5203,8 @@
         </is>
       </c>
       <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr">
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr">
         <is>
           <t>Google is searching us</t>
         </is>
@@ -5130,7 +5251,8 @@
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr"/>
-      <c r="M100" t="inlineStr">
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr">
         <is>
           <t>New Britain Mask</t>
         </is>
@@ -5177,7 +5299,8 @@
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr">
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr">
         <is>
           <t>Golden Snub-Nosed Monkey</t>
         </is>
@@ -5224,7 +5347,8 @@
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr"/>
-      <c r="M102" t="inlineStr">
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr">
         <is>
           <t>Loris</t>
         </is>
@@ -5271,7 +5395,8 @@
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr"/>
-      <c r="M103" t="inlineStr">
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr">
         <is>
           <t>Japanese Macaque</t>
         </is>
@@ -5318,7 +5443,8 @@
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr"/>
-      <c r="M104" t="inlineStr">
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr">
         <is>
           <t>Llama</t>
         </is>
@@ -5365,7 +5491,8 @@
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
-      <c r="M105" t="inlineStr">
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr">
         <is>
           <t>Red Fox</t>
         </is>
@@ -5412,7 +5539,8 @@
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
-      <c r="M106" t="inlineStr">
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr">
         <is>
           <t>Songye Kifwebe Mask</t>
         </is>
@@ -5459,7 +5587,8 @@
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
-      <c r="M107" t="inlineStr">
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr">
         <is>
           <t>Bemba Mask</t>
         </is>
@@ -5506,7 +5635,8 @@
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
-      <c r="M108" t="inlineStr">
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr">
         <is>
           <t>Elema Mask</t>
         </is>
@@ -5553,7 +5683,8 @@
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
-      <c r="M109" t="inlineStr">
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr">
         <is>
           <t>Sepik River Mask</t>
         </is>
@@ -5600,7 +5731,8 @@
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
-      <c r="M110" t="inlineStr">
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr">
         <is>
           <t>Palm Peach Mask</t>
         </is>
@@ -5647,7 +5779,8 @@
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr">
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr">
         <is>
           <t>Indonesian Mask</t>
         </is>
@@ -5694,7 +5827,8 @@
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
-      <c r="M112" t="inlineStr">
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr">
         <is>
           <t>Philippine Eagle</t>
         </is>
@@ -5741,7 +5875,8 @@
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
-      <c r="M113" t="inlineStr">
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr">
         <is>
           <t>Puma</t>
         </is>
@@ -5788,7 +5923,8 @@
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
-      <c r="M114" t="inlineStr">
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr">
         <is>
           <t>Sifaka</t>
         </is>
@@ -5835,7 +5971,8 @@
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
-      <c r="M115" t="inlineStr">
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr">
         <is>
           <t>Fennec Fox</t>
         </is>
@@ -5882,7 +6019,8 @@
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
-      <c r="M116" t="inlineStr">
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr">
         <is>
           <t>Dolphin</t>
         </is>
@@ -5939,6 +6077,11 @@
       <c r="L117" t="inlineStr"/>
       <c r="M117" t="inlineStr">
         <is>
+          <t>Dr. Alan Grant, Jurassic Park III</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
           <t>"Reverse Darwinism:
  Survival of the most idiotic"</t>
         </is>
@@ -5993,7 +6136,8 @@
         </is>
       </c>
       <c r="L118" t="inlineStr"/>
-      <c r="M118" t="inlineStr">
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr">
         <is>
           <t>Chicken Heart</t>
         </is>
@@ -6048,7 +6192,8 @@
         </is>
       </c>
       <c r="L119" t="inlineStr"/>
-      <c r="M119" t="inlineStr">
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr">
         <is>
           <t>Everything Fist Well</t>
         </is>
@@ -6105,6 +6250,11 @@
       <c r="L120" t="inlineStr"/>
       <c r="M120" t="inlineStr">
         <is>
+          <t>Antoine de Saint-Exupery, The Little Prince.</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
           <t>VISIBLE TO ME
  "What is essential is invisible to the eye"</t>
         </is>
@@ -6155,7 +6305,8 @@
       </c>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr"/>
-      <c r="M121" t="inlineStr">
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr">
         <is>
           <t>Crystal Meth Clear</t>
         </is>
@@ -6206,7 +6357,8 @@
       </c>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
-      <c r="M122" t="inlineStr">
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr">
         <is>
           <t>Iceberg</t>
         </is>
@@ -6261,7 +6413,8 @@
         </is>
       </c>
       <c r="L123" t="inlineStr"/>
-      <c r="M123" t="inlineStr">
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr">
         <is>
           <t>Corazón Espinado</t>
         </is>
@@ -6312,7 +6465,8 @@
       </c>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
-      <c r="M124" t="inlineStr">
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr">
         <is>
           <t>Heartless</t>
         </is>
@@ -6367,7 +6521,8 @@
         </is>
       </c>
       <c r="L125" t="inlineStr"/>
-      <c r="M125" t="inlineStr">
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" t="inlineStr">
         <is>
           <t>Under the reign of king Minos</t>
         </is>
@@ -6423,7 +6578,8 @@
         </is>
       </c>
       <c r="L126" t="inlineStr"/>
-      <c r="M126" t="inlineStr">
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr">
         <is>
           <t>YUKO SHIMIZU: CONTEMPORARY HEROINES
  How to combine Japanese and American illustration?
@@ -6503,7 +6659,8 @@
           <t>Animal</t>
         </is>
       </c>
-      <c r="M127" t="inlineStr">
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr">
         <is>
           <t>BLINDNESS
  I know the reason why you hate so much this kind of place,
@@ -6572,7 +6729,8 @@
           <t>Animal</t>
         </is>
       </c>
-      <c r="M128" t="inlineStr">
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr">
         <is>
           <t>SELF-DESTRUCTIVE
  Your portraits are getting outdated
@@ -6643,7 +6801,8 @@
           <t>Counterfeit</t>
         </is>
       </c>
-      <c r="M129" t="inlineStr">
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr">
         <is>
           <t>TRIGGER
  Pain, has many names,
@@ -6707,7 +6866,8 @@
           <t>Counterfeit</t>
         </is>
       </c>
-      <c r="M130" t="inlineStr">
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr">
         <is>
           <t>ARMORED HEART
  If you were hurt,
@@ -6771,7 +6931,8 @@
           <t>Collateral</t>
         </is>
       </c>
-      <c r="M131" t="inlineStr">
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr">
         <is>
           <t>NATIVE
  Monocultures monotonize-us,
@@ -6832,7 +6993,8 @@
           <t>Collateral</t>
         </is>
       </c>
-      <c r="M132" t="inlineStr">
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr">
         <is>
           <t>UNINTENDED PERMANENCE
  Every character need to be shaken
@@ -6900,7 +7062,8 @@
       </c>
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr"/>
-      <c r="M133" t="inlineStr">
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" t="inlineStr">
         <is>
           <t>Lossing weight</t>
         </is>
@@ -6955,7 +7118,8 @@
         </is>
       </c>
       <c r="L134" t="inlineStr"/>
-      <c r="M134" t="inlineStr">
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr">
         <is>
           <t>Native</t>
         </is>
@@ -7006,7 +7170,8 @@
       </c>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
-      <c r="M135" t="inlineStr">
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr">
         <is>
           <t>Frog You!</t>
         </is>
@@ -7049,7 +7214,8 @@
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr"/>
-      <c r="M136" t="inlineStr">
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr">
         <is>
           <t>"Wellness only operates under your presence"</t>
         </is>
@@ -7092,7 +7258,8 @@
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
-      <c r="M137" t="inlineStr">
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr">
         <is>
           <t>🤖👽💀
  "Automatically Alienated to you until Dead"</t>
@@ -7136,7 +7303,8 @@
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr"/>
-      <c r="M138" t="inlineStr">
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr">
         <is>
           <t>"You don't have limits when you are on heels"</t>
         </is>
@@ -7181,6 +7349,11 @@
       <c r="L139" t="inlineStr"/>
       <c r="M139" t="inlineStr">
         <is>
+          <t>Kwon-taek</t>
+        </is>
+      </c>
+      <c r="N139" t="inlineStr">
+        <is>
           <t>PAINTED FIRE
  Kwon-taek (2002)
  He painted her like a swan

</xml_diff>